<commit_message>
Added calculations for corn belt and estimation extra factors
</commit_message>
<xml_diff>
--- a/Decoupling/Sample table.xlsx
+++ b/Decoupling/Sample table.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="65" documentId="8_{96144072-B6CB-4274-8A9F-FA430C65C366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1634F789-A854-42BE-845E-D580A0256DAA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F9967E14-FE80-435C-8D26-33B0FB464AE3}"/>
+    <workbookView minimized="1" xWindow="2240" yWindow="1810" windowWidth="14400" windowHeight="7360" xr2:uid="{F9967E14-FE80-435C-8D26-33B0FB464AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,13 +212,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800413E4-B40A-4233-ACA2-1D09AD6DC4D8}">
   <dimension ref="A1:U71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D62" sqref="B62:D62"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -551,29 +551,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="26" x14ac:dyDescent="0.6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C2" s="5"/>
@@ -597,39 +597,39 @@
       <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="11" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11" t="s">
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11" t="s">
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11" t="s">
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -3523,6 +3523,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009AA21861009F844A94D45FCCECE366B4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e658606205e1dbc8e3f5b77287602906">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c03d4cec-2a4e-42ae-b684-cd712438aa88" xmlns:ns4="8e23d785-2c7b-4ebd-b19b-adb2653ad200" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7ada76741c526a1ec7a93ee9c23d7ee" ns3:_="" ns4:_="">
     <xsd:import namespace="c03d4cec-2a4e-42ae-b684-cd712438aa88"/>
@@ -3745,22 +3760,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D69E1FF-5BA1-4AB0-BD17-E2AD77484D3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF5ECB8-0D28-4E9B-96AF-D048046DE127}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F53DE65A-C600-49B7-A984-B249899E3455}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3777,21 +3794,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF5ECB8-0D28-4E9B-96AF-D048046DE127}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D69E1FF-5BA1-4AB0-BD17-E2AD77484D3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update accompanying files for first complete version
</commit_message>
<xml_diff>
--- a/Decoupling/Sample table.xlsx
+++ b/Decoupling/Sample table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/ensxvd_mail_missouri_edu/Documents/FAPRI/MarketResearch/Decoupling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="8_{96144072-B6CB-4274-8A9F-FA430C65C366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FCB6A47-A28E-453C-86E3-691D498EB17C}"/>
+  <xr:revisionPtr revIDLastSave="252" documentId="8_{96144072-B6CB-4274-8A9F-FA430C65C366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C104FA60-FC9C-4C40-97D4-8EDE37AE0024}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2580" yWindow="2150" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{F9967E14-FE80-435C-8D26-33B0FB464AE3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F9967E14-FE80-435C-8D26-33B0FB464AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -326,16 +326,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -669,29 +669,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="26" x14ac:dyDescent="0.6">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C2" s="5"/>
@@ -718,36 +718,36 @@
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15" t="s">
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15" t="s">
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15" t="s">
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -3644,8 +3644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D4A451-9A48-4606-884A-C03A7DCBDC54}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:D31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3678,18 +3678,18 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="16">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="16">
         <v>81</v>
       </c>
     </row>
@@ -3697,18 +3697,18 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>81</v>
       </c>
     </row>
@@ -3716,18 +3716,18 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <v>81</v>
       </c>
     </row>
@@ -3740,26 +3740,26 @@
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="16">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="16">
         <v>19</v>
       </c>
       <c r="F14" t="s">
@@ -3767,10 +3767,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="16">
         <v>81</v>
       </c>
     </row>
@@ -3778,18 +3778,18 @@
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="16">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="16">
         <v>81</v>
       </c>
     </row>
@@ -3797,26 +3797,26 @@
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="16">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="16">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="16">
         <v>81</v>
       </c>
     </row>
@@ -3824,10 +3824,10 @@
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="16">
         <v>81</v>
       </c>
     </row>
@@ -3840,10 +3840,10 @@
       <c r="B28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="16">
         <v>81</v>
       </c>
       <c r="F28" t="s">
@@ -3854,10 +3854,10 @@
       <c r="B31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="16" t="s">
         <v>48</v>
       </c>
       <c r="F31" t="s">
@@ -3873,10 +3873,10 @@
       <c r="B34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="16" t="s">
         <v>50</v>
       </c>
       <c r="F34" t="s">
@@ -3904,7 +3904,7 @@
       <c r="F41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G41" s="16">
+      <c r="G41" s="14">
         <v>1</v>
       </c>
       <c r="H41" s="12">
@@ -4034,12 +4034,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4266,15 +4263,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF5ECB8-0D28-4E9B-96AF-D048046DE127}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D69E1FF-5BA1-4AB0-BD17-E2AD77484D3B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4299,10 +4300,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D69E1FF-5BA1-4AB0-BD17-E2AD77484D3B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF5ECB8-0D28-4E9B-96AF-D048046DE127}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>